<commit_message>
Sesión 2 - Caso 1
</commit_message>
<xml_diff>
--- a/datasets/venta_productos.xlsx
+++ b/datasets/venta_productos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\datascience-intermediate-cenace-2024\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCCE1FF-0AAB-4425-8053-21355D0E741F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED40802B-AABE-456C-9505-58DE13486894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37680" yWindow="4005" windowWidth="29040" windowHeight="15720" xr2:uid="{DF050E0C-9468-41EB-BD0E-E3D3BD593B76}"/>
+    <workbookView xWindow="37680" yWindow="4005" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="9" xr2:uid="{DF050E0C-9468-41EB-BD0E-E3D3BD593B76}"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCTOS" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,11 @@
     <sheet name="PAGOS" sheetId="8" r:id="rId8"/>
     <sheet name="CANCELACIONES" sheetId="9" r:id="rId9"/>
     <sheet name="Hoja10" sheetId="10" r:id="rId10"/>
+    <sheet name="Hoja11" sheetId="11" r:id="rId11"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Hoja10!$C$2:$G$2</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="55">
   <si>
     <t>PRODUCTO</t>
   </si>
@@ -207,6 +211,9 @@
   </si>
   <si>
     <t>PACO@BIMBO.COM</t>
+  </si>
+  <si>
+    <t>PRECIO</t>
   </si>
 </sst>
 </file>
@@ -217,7 +224,7 @@
     <numFmt numFmtId="166" formatCode="d/m/yyyy\ hh:mm:ss\ AM/PM"/>
     <numFmt numFmtId="168" formatCode="_-[$$-80A]* #,##0.00_-;\-[$$-80A]* #,##0.00_-;_-[$$-80A]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +242,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -261,18 +276,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="27" formatCode="d/m/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="d/m/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="d/m/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="_-[$$-80A]* #,##0.00_-;\-[$$-80A]* #,##0.00_-;_-[$$-80A]* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="_-[$$-80A]* #,##0.00_-;\-[$$-80A]* #,##0.00_-;_-[$$-80A]* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="_-[$$-80A]* #,##0.00_-;\-[$$-80A]* #,##0.00_-;_-[$$-80A]* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="d/m/yyyy\ hh:mm:ss\ AM/PM"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -283,6 +322,132 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5C61D0C6-B16F-48AA-A630-ABA26440FD6F}" name="TablaProductos" displayName="TablaProductos" ref="A1:D6" totalsRowShown="0">
+  <autoFilter ref="A1:D6" xr:uid="{5C61D0C6-B16F-48AA-A630-ABA26440FD6F}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{933C579D-1819-4B01-A718-969ECFDAB097}" name="PRODUCTO"/>
+    <tableColumn id="2" xr3:uid="{9BC36082-72B9-4542-9808-A0A1215788C5}" name="NOMBRE"/>
+    <tableColumn id="3" xr3:uid="{89753E66-BAA1-461A-A691-169A4AF2875D}" name="CATEGORIA"/>
+    <tableColumn id="4" xr3:uid="{7470A5D0-3369-4DED-B829-E8D9D3C0BE0B}" name="DEPARTAMENTO"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3891D25-EBB7-4DF9-BCB9-2F617A6E1F67}" name="TablaListadoPrecios" displayName="TablaListadoPrecios" ref="A1:F4" totalsRowShown="0">
+  <autoFilter ref="A1:F4" xr:uid="{C3891D25-EBB7-4DF9-BCB9-2F617A6E1F67}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{8FF7E838-C64A-4168-A73A-A68066D8BBF2}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{C18688E2-58CA-4935-8497-72E674D19FC9}" name="PRODUCTO"/>
+    <tableColumn id="3" xr3:uid="{737DFD18-5F7A-4C2B-B7F1-E8D2B18759A5}" name="FECHA" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{329BD726-D314-45EB-AF01-FC7949D938C9}" name="PRECIO_LISTA" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{9ED82AA8-8193-42AC-B6F0-695A06B0482D}" name="DESCUENTO" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{F7EC7F24-F98C-438B-AF5E-47C047ED9822}" name="PRECIO_VENTA" dataDxfId="3">
+      <calculatedColumnFormula>(D2-E2)*1.16</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C081100D-131A-4CD7-8C9E-240C06E66969}" name="TablaAlmacenes" displayName="TablaAlmacenes" ref="A1:E2" totalsRowShown="0">
+  <autoFilter ref="A1:E2" xr:uid="{C081100D-131A-4CD7-8C9E-240C06E66969}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{6437BB13-63C8-4B3C-9053-5DAF0FC713C7}" name="ALMACEN"/>
+    <tableColumn id="2" xr3:uid="{E9F36675-30B8-407D-ADC4-D5F37CBE411A}" name="NOMBRE"/>
+    <tableColumn id="3" xr3:uid="{AD2C1DC8-AF41-4B62-B67E-99037E29F059}" name="DIRECCION"/>
+    <tableColumn id="4" xr3:uid="{C87D9AB1-5206-4DB9-8A4F-D0DD07269691}" name="LATITUD"/>
+    <tableColumn id="5" xr3:uid="{4E6F9B43-F97A-4A89-9130-CD58A810638D}" name="LONGITUD"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{22DB0DF2-C896-4908-8356-BA2E43149E69}" name="TablaProductoAlmacen" displayName="TablaProductoAlmacen" ref="A1:G3" totalsRowShown="0">
+  <autoFilter ref="A1:G3" xr:uid="{22DB0DF2-C896-4908-8356-BA2E43149E69}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{6CF102FD-A2A9-4D4B-A4EB-AA01F97D9EBC}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{3759A277-6AD6-428E-A3F1-7324F73CC03D}" name="ALMACEN"/>
+    <tableColumn id="3" xr3:uid="{A7455A7F-250B-45FE-9F2D-A0B5C0BE414B}" name="PRODUCTO"/>
+    <tableColumn id="4" xr3:uid="{2FD23B6B-522F-47E3-A6F5-D80A375847A9}" name="ZONA"/>
+    <tableColumn id="5" xr3:uid="{911027AB-51B1-44FA-8089-1FE62BD0F45B}" name="ESTANTE"/>
+    <tableColumn id="6" xr3:uid="{1A8A5C9E-88A0-4C35-B255-C2E94A37EF87}" name="NUMERO"/>
+    <tableColumn id="7" xr3:uid="{3E4A603E-DCAD-4A33-A0C5-0EA45F981208}" name="CANTIDAD"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CA9DF06A-EBCB-4323-9507-E929314CAE73}" name="TablaVentas" displayName="TablaVentas" ref="A1:D2" totalsRowShown="0">
+  <autoFilter ref="A1:D2" xr:uid="{CA9DF06A-EBCB-4323-9507-E929314CAE73}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{688E839A-2269-46C0-9045-A2A8D5E06AA9}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{5D75641D-926A-4547-A9A1-0FC3C985D037}" name="VENDEDOR"/>
+    <tableColumn id="3" xr3:uid="{D7F9E280-F8A3-4908-9560-E3B16464177D}" name="FECHA_ABRE" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{C968784D-7FF1-4A6E-B54D-F59E464DB223}" name="FECHA_CIERRA" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{81C8C4B1-03FE-4E0A-A0C1-C76ABE4152FA}" name="TablaProductoVenta" displayName="TablaProductoVenta" ref="A1:C21" totalsRowShown="0">
+  <autoFilter ref="A1:C21" xr:uid="{81C8C4B1-03FE-4E0A-A0C1-C76ABE4152FA}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{93439BDC-2C8F-439A-AA53-D1031C1E2488}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{F7010216-7BC4-491E-AB5B-917259874A61}" name="VENTA"/>
+    <tableColumn id="3" xr3:uid="{56698CE5-861A-42EA-B49E-E8941D432044}" name="PRODUCTO"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1C86BA22-DA0A-4844-921C-565C7B82D440}" name="TablaVendedores" displayName="TablaVendedores" ref="A1:C3" totalsRowShown="0">
+  <autoFilter ref="A1:C3" xr:uid="{1C86BA22-DA0A-4844-921C-565C7B82D440}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{86C2A530-AD21-4A6B-BF52-3801236F9E30}" name="VENDEDOR"/>
+    <tableColumn id="2" xr3:uid="{0D0D9848-459C-48F7-A3BD-3EAA5FF82277}" name="NOMBRE"/>
+    <tableColumn id="3" xr3:uid="{2A660ED0-DAAF-4BB1-98D9-1ADAD135C940}" name="CORREO" dataCellStyle="Hipervínculo"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9084358A-57B6-4663-8EFD-545141D83F00}" name="TablaPagos" displayName="TablaPagos" ref="A1:F2" totalsRowShown="0">
+  <autoFilter ref="A1:F2" xr:uid="{9084358A-57B6-4663-8EFD-545141D83F00}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{D43CD172-9532-4378-AB75-8EB0A7600D52}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{24272F09-390D-4A0D-90A3-DE7BA63E957F}" name="VENTA"/>
+    <tableColumn id="3" xr3:uid="{F07620A7-2AF6-42F9-B40D-B2EABE033D27}" name="TOTAL"/>
+    <tableColumn id="4" xr3:uid="{63117754-79F5-48A9-80FC-7CE925CDF490}" name="MONTO_PAGADO"/>
+    <tableColumn id="5" xr3:uid="{925F0687-A5E4-4012-93FB-55D0EC0C463D}" name="MONTO_DEVUELTO">
+      <calculatedColumnFormula>D2-C2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{06F9C906-9D63-433E-BA1D-BACD273A0BAF}" name="FECHA" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{B3C2D46C-194F-4992-9C3B-4B575EDA1275}" name="TablaCancelaciones" displayName="TablaCancelaciones" ref="A1:C2" totalsRowShown="0">
+  <autoFilter ref="A1:C2" xr:uid="{B3C2D46C-194F-4992-9C3B-4B575EDA1275}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{B9D841A7-E025-44E1-A2C3-058686E5C4C6}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{5A788F48-AA1D-4AA1-A19A-0859081BCBC1}" name="VENTA"/>
+    <tableColumn id="3" xr3:uid="{E3A58D53-F7EA-4448-979D-021AB7F5ED8E}" name="SUPERVISOR"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -602,15 +767,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE375158-F3FF-4F58-818D-CB64CC74D98F}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="12.81640625" customWidth="1"/>
     <col min="2" max="2" width="19.6328125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="23.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -698,13 +865,115 @@
         <v>18</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D13" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5396F9-4BB3-4F94-8903-B6F0D42F36B6}">
+  <dimension ref="C1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="11.7265625" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="F1"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="6">
+        <v>45436.772557870368</v>
+      </c>
+      <c r="G3" s="3">
+        <v>20.88</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="6">
+        <v>45435.647557870368</v>
+      </c>
+      <c r="G4" s="3">
+        <v>24.36</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="6">
+        <v>45435.647557870368</v>
+      </c>
+      <c r="G5" s="3">
+        <v>22.445999999999994</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="C2:G2" xr:uid="{EB5396F9-4BB3-4F94-8903-B6F0D42F36B6}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:G5">
+      <sortCondition descending="1" ref="F2"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED74E9CC-3E6B-4B24-B72F-916CC5FF8A6E}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -720,11 +989,12 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="12.81640625" customWidth="1"/>
     <col min="3" max="3" width="29.26953125" customWidth="1"/>
     <col min="4" max="4" width="17.453125" customWidth="1"/>
     <col min="5" max="5" width="15.7265625" customWidth="1"/>
@@ -816,6 +1086,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -824,10 +1097,15 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.36328125" customWidth="1"/>
+    <col min="3" max="3" width="13.08984375" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -865,6 +1143,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -873,10 +1154,15 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="11.36328125" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -950,6 +1236,9 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -958,13 +1247,14 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="12.81640625" customWidth="1"/>
     <col min="3" max="3" width="17.26953125" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" customWidth="1"/>
+    <col min="4" max="4" width="16.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -997,6 +1287,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1005,10 +1298,13 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection sqref="A1:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="12.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1244,6 +1540,9 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1252,11 +1551,12 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="12.81640625" customWidth="1"/>
     <col min="3" max="3" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1299,6 +1599,9 @@
     <hyperlink ref="C3" r:id="rId2" xr:uid="{A5B613FA-A82F-4F3F-B076-7BFF71E43C45}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1307,12 +1610,13 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="17.90625" customWidth="1"/>
+    <col min="4" max="4" width="17.6328125" customWidth="1"/>
+    <col min="5" max="5" width="19.36328125" customWidth="1"/>
     <col min="6" max="6" width="16.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1359,6 +1663,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1367,10 +1674,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="13.90625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1396,5 +1706,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>